<commit_message>
updating final project files
</commit_message>
<xml_diff>
--- a/final-project-files/npr-data/npr-data-winter2019.xlsx
+++ b/final-project-files/npr-data/npr-data-winter2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahpearman/Documents/data-stories/final-project-files/npr-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9375D180-2286-0146-AD18-28FDC9AE50E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42841ED0-C111-2044-824F-BF5D29395FD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{E79CF531-6F6B-8A42-9F6F-6FDF6B3FECB5}"/>
   </bookViews>
@@ -35,18 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Jan 2017</t>
-  </si>
-  <si>
-    <t>Dec 2017</t>
-  </si>
-  <si>
-    <t>Dec 2018</t>
-  </si>
-  <si>
-    <t>Dec 2019</t>
-  </si>
-  <si>
     <t>Number of smart speakers in US households</t>
   </si>
   <si>
@@ -54,6 +42,18 @@
   </si>
   <si>
     <t>% of U.S. adults who own smart speakers</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
   </si>
 </sst>
 </file>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811EED69-D4D1-1945-9DFF-CABCF0C6F46A}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -418,62 +418,59 @@
     <col min="4" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2">
+        <v>67000000</v>
+      </c>
+      <c r="D2">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2">
+        <v>119000000</v>
+      </c>
+      <c r="D3">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>21</v>
-      </c>
-      <c r="E2">
+      <c r="B4">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2">
-        <v>67000000</v>
-      </c>
-      <c r="D3" s="2">
-        <v>119000000</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="C4" s="2">
         <v>157000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>1.7</v>
-      </c>
       <c r="D4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E4">
         <v>2.6</v>
       </c>
     </row>

</xml_diff>